<commit_message>
amazon and mynthra added
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,25 +446,25 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pesado</t>
+          <t>LEE TEX</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Men Slim Fit Beige Lycra Blend Trousers</t>
+          <t>Women Regular Fit Black Cotton Blend Trousers</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>489</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -473,209 +473,209 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Women Regular Fit Black, Light Green Cotton Blend Trousers</t>
+          <t>Women Regular Fit Maroon Cotton Blend Trousers</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>649</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Roadster</t>
+          <t>POPWINGS</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Men Regular Fit Grey Cotton Blend Trousers</t>
+          <t>Women Regular Fit Multicolor Viscose Rayon Trousers</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>787</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>PETER ENGLAND</t>
+          <t>GRECIILOOKS</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Men Slim Fit Black Cotton Blend Trousers</t>
+          <t>Women's Yoga Dress Pants Stretchy Work Slacks Business Casual Office Straight Leg/Boot-Cut Elastic Waist Regular Fit Trouser Pant (XS, Green) (XS, Pink)</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1259</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>135</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Raymond</t>
+          <t>NEMO FASHION</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Men Slim Fit Black Viscose Rayon Trousers</t>
+          <t>Premium Polyester Men’s Jogger Regular Fit Track Pants for Men, Stretchable Joggers, Gym, Sports, and Yoga Wear.</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>944</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PETER ENGLAND</t>
+          <t>KOTTY</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Men Slim Fit Grey Polyester Viscose Blend Trousers</t>
+          <t>Women Polyester Blend Green Solid Trousers</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1169</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>131</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>U.S. POLO ASSN.</t>
+          <t>AVOLT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Men Slim Fit Multicolor Cotton Blend Trousers</t>
+          <t>Dry Fit Track Pants Combo I Slim Fit Sports Track Pants</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1481</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>PARK AVENUE</t>
+          <t>Cloth Theory</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Men Regular Fit Blue Cotton Blend Trousers</t>
+          <t>Boy's Regular Track Pants</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1449</v>
+        <v>379</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Roadster</t>
+          <t>KOTTY</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Men Regular Fit Grey Pure Cotton Trousers</t>
+          <t>Women Regular Fit Black Viscose Rayon Trousers</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1649</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Foxter</t>
+          <t>KOTTY</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Pack of 2 Women Regular Fit Multicolor Cotton Blend Trousers</t>
+          <t>Women Regular Fit Black Viscose Rayon Trousers</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>699</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>LEE TEX</t>
+          <t>KOTTY</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Women Regular Fit Black, White Cotton Blend Trousers</t>
+          <t>Women Regular Fit Dark Green Viscose Rayon Trousers</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>649</v>
+        <v>381</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>LEE TEX</t>
+          <t>JUGULAR</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Pack of 2 Women Regular Fit Maroon Cotton Blend Trousers</t>
+          <t>Men's Slim Fit Cotton Track Pant</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>449</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KOTTY</t>
+          <t>POPWINGS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Women Regular Fit Black Viscose Rayon Trousers</t>
+          <t>Women Relaxed Brown Polycotton Trousers</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>399</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15">
@@ -684,12 +684,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>KOTTY</t>
+          <t>ADDYVERO</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Women Regular Fit Dark Green Viscose Rayon Trousers</t>
+          <t>Women Regular Fit Black Cotton Blend Trousers</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -698,128 +698,128 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Foxter</t>
+          <t>CYPHUS</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Pack of 2 Women Regular Fit Multicolor Cotton Blend Trousers</t>
+          <t>Men Regular Fit Black Cotton Blend Trousers</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>699</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SASSAFRAS</t>
+          <t>CYPHUS</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Women Relaxed Pink Cotton Blend Trousers</t>
+          <t>Men Regular Fit Cream Cotton Blend Trousers</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>674</v>
+        <v>399</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>129</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>PARK AVENUE</t>
+          <t>TOPLOT</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Men Relaxed Grey Crepe Trousers</t>
+          <t>Men's Regular Fit Trackpant (Track-Pant-5070)</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>720</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LEE TEX</t>
+          <t>CYPHUS</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Pack of 2 Women Regular Fit Purple, Blue Cotton Blend Trousers</t>
+          <t>Men Regular Fit Grey Cotton Blend Trousers</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>449</v>
+        <v>399</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>LEE TEX</t>
+          <t>ENDEAVOUR WEAR</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Women Regular Fit Black Cotton Blend Trousers</t>
+          <t>Men's Regular Fit Trackpants</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>292</v>
+        <v>399</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>PUMA</t>
+          <t>KOTTY</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Men Solid Grey Track Pants</t>
+          <t>Women Regular Fit Brown Cotton Blend Trousers</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1624</v>
+        <v>399</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PARK AVENUE</t>
+          <t>FRANKO ROGER</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Men Regular Fit Beige Cotton Blend Trousers</t>
+          <t>Men Slim Fit Black Viscose Rayon Trousers</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>1249</v>
+        <v>413</v>
       </c>
     </row>
     <row r="23">
@@ -828,340 +828,2302 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>PARK AVENUE</t>
+          <t>ELANHOOD</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Men Black Viscose Rayon Trousers</t>
+          <t>Men Regular Fit Black Cotton Blend Trousers</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>919</v>
+        <v>419</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Urbano Fashion</t>
+          <t>JPM brothers</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Men Slim Fit Grey Cotton Blend Trousers</t>
+          <t>Mens Regular Fit Lycra Pant</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>649</v>
+        <v>429</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LEVI'S</t>
+          <t>AKIKO</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Men Regular Fit Green Pure Cotton Trousers</t>
+          <t>Women Regular Fit White Cotton Blend Trousers</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1484</v>
+        <v>439</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Raymond</t>
+          <t>Amazon Brand - Symbol</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Men Slim Fit Black Viscose Rayon Trousers</t>
+          <t>Men's Regular Track Pants</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>1049</v>
+        <v>439</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CYPHUS</t>
+          <t>DBURKE</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Men Regular Fit Black Cotton Blend Trousers</t>
+          <t>Track Pants for Mens Track Pants Men Track Pants for Mens Sports Sports Track Pants Lower for Mens and Women</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>399</v>
+        <v>472</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>LEE TEX</t>
+          <t>Aahwan</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Women Regular Fit Black Cotton Blend Trousers</t>
+          <t>Women's &amp; Girls' Solid Split Hem Flare Leg Pants Trouser</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>399</v>
+        <v>474</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>PARK AVENUE</t>
+          <t>BLUE STAR SHARK</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Men Regular Fit Khaki Cotton Blend Trousers</t>
+          <t>Men's Lycra Stretchable Regular Fit Joggers Navy Track Pant Lower</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1499</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>28</v>
+        <v>97</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Highlander</t>
+          <t>JUGULAR</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Men Slim Fit White Cotton Blend Trousers</t>
+          <t>Men's Slim Fit Track pants</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>712</v>
+        <v>479</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SASSAFRAS</t>
+          <t>Laabha</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Women Relaxed Light Green Cotton Blend Trousers</t>
+          <t>Solid Track Pants</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>674</v>
+        <v>489</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>PARK AVENUE</t>
+          <t>Laabha</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Men Slim Fit Grey Polycotton Trousers</t>
+          <t>Solid Track Pants</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1099</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Tokyo Talkies</t>
+          <t>Hubberholme</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Women Regular Fit Light Blue Polycotton Trousers</t>
+          <t>Men Track Pants</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>404</v>
+        <v>493</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>KOTTY</t>
+          <t>ENDEAVOUR WEAR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Women Regular Fit Dark Green Viscose Rayon Trousers</t>
+          <t>Men's Regular Fit Trackpants</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>399</v>
+        <v>499</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>33</v>
+        <v>130</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>KOTTY</t>
+          <t>Majestic Man</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Women Regular Fit Green Viscose Rayon Trousers</t>
+          <t>Slim Fit Formal Trousers for Men</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>399</v>
+        <v>499</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>34</v>
+        <v>102</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Q-Rious</t>
+          <t>Chromozome</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Women Regular Fit White Cotton Blend Trousers</t>
+          <t>Men Slim Fit Polyester, Cotton Track Pant</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>399</v>
+        <v>499</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>35</v>
+        <v>138</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>LEE TEX</t>
+          <t>Generic</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Women Regular Fit Maroon Cotton Blend Trousers</t>
+          <t>Aruljohti Knits Men's Casual Pant/Sweat Pant/Jogger/Track Pant Cotton Solid Designer Regular Fit Track Pants</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>292</v>
+        <v>499</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>36</v>
+        <v>141</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>PARK AVENUE</t>
+          <t>Chromozome</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Men Regular Fit Dark Blue Viscose Rayon Trousers</t>
+          <t>Men's Regular Fit Cotton Track Pants</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1959</v>
+        <v>499</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>37</v>
+        <v>114</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>PARK AVENUE</t>
+          <t>Amazon Brand - Symbol</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Men Skinny Fit Green Cotton Blend Trousers</t>
+          <t>Men's Slim Dress Pants</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1649</v>
+        <v>517</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>KOTTY</t>
+          <t>Enamor</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Women Regular Fit Black Viscose Rayon Trousers</t>
+          <t>Essentials E066 Cotton Lounge Jogger for Women</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>399</v>
+        <v>519</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Hubberholme</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Men's Relaxed Track Pants</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Enamor</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Essentials Women's Mid Rise Crop Length Soft &amp; Drapey Stretch Viscose Culottes with Smart Side Slits - E064</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Enamor</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Essentials E060 Women’s Slim Fit Terry Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Men's Slim Casual Trousers</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Tokyo Talkies</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Women Tapered Blue Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Alan Jones Clothing</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Men's Slim Fit Track pants</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Okane</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Men Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Okane</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Men Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>plusS</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Women Track Pants</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>plusS</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Women Track Pants</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Men's Slim Casual Pants</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Chromozome</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Men's Regular Fit Cotton Track Pants</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Peppyzone</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Men's Camouflage Regular Fit Track Pant</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>LEE TEX</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Women Regular Fit Black, White Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>SASSAFRAS</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Women Relaxed Black Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Men's Slim Fit Formal Trousers</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>MARK LOUIIS</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Men's Regular Fit Track pants</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Smarty Pants</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Women Floral Printed Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>T2F</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Boys Printed Track Pants (Pack of 5)</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Urbano Fashion</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Purple Pure Cotton Trousers</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Smarty Pants</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Women Cotton Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Smarty Pants</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Women Cotton Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Smarty Pants</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Women Cotton Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Zivame</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Neostreak</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Men's Slim Fit Jeans</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SASSAFRAS</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Women Relaxed Pink Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Chromozome</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Men's Regular Fit Track Pants</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Men's Slim Fit Stretchable Jeans</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Foxter</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Pack of 2 Women Regular Fit Multicolor Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Women Track Pants</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Men's Regular Casual Trousers</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Men's Straight Casual Trousers</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Van Heusen</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Athleisure Stretch Lounge Pants With Pockets</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>0-DEGREE</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Black Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Inkast Denim Co.</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Men's Regular Casual Trousers</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Roadster</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Beige Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Smarty Pants</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Women 2-Pcs Printed Night suit</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Smarty Pants</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Women 2-Pcs Printed Night suit</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Whitewhale</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Men's Loose Fit Cotton Trousers</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>MAYSIXTY</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Printed Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>MAYSIXTY</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Printed Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>9rasa</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Cotton Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Men's Slim Fit Formal Trousers</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>MAYSIXTY</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Printed Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>HIGHLANDER</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Men Regular Fit Black Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Men's Slim Casual Trousers</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Men Stretch Casual Trouser</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>plusS</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Women Track Pants</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Enamor</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Essentials Women's Mid Rise Slim Fit Straight Leg Breathable Stretch Cotton Lounge Pants with Drawstring and Invisible Zipper Pockets- E014</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Men's Flexi Waist Slim Casual Pants</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Symbol</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Men's Flexi Waist Slim Casual Pants</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>FLYING MACHINE</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Men Solid Black Track Pants</t>
+        </is>
+      </c>
+      <c r="D93" t="n">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Hancock</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Checked Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Hancock</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Checked Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Hancock</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Checked Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Van Heusen</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Men's Track Pants</t>
+        </is>
+      </c>
+      <c r="D97" t="n">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Gallus</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>PARK AVENUE</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Men Regular Fit Brown Viscose Rayon Trousers</t>
+        </is>
+      </c>
+      <c r="D99" t="n">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>SIAPA</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Amazon Brand - Inkast Denim Co.</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Men's Slim Fit Casual Pants</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>SOJANYA</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Men Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>SOJANYA</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Men Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>PUMA</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Men Solid Black Track Pants</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>1624</v>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>SOJANYA</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Men Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D104" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>SOJANYA</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Men Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>SOJANYA</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Men Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D106" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>SOJANYA</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Men Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D107" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>SOJANYA</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Men Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D108" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>SOJANYA</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Men Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D109" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>SOJANYA</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Men Dhoti Pants</t>
+        </is>
+      </c>
+      <c r="D110" t="n">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>McHenry</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Men's Solid Formal Regular Fit Wrinkle Free PolyViscose Trousers</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>NAUTICA</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Men Solid Grey Track Pants</t>
+        </is>
+      </c>
+      <c r="D112" t="n">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Jockey</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Men's Cotton Track Pants</t>
+        </is>
+      </c>
+      <c r="D113" t="n">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Raymond</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Black Viscose Rayon Trousers</t>
+        </is>
+      </c>
+      <c r="D114" t="n">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>PETER ENGLAND</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Dark Green Pure Cotton Trousers</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Zivame</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Women Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>PETER ENGLAND</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Dark Blue Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Van Heusen</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Athleisure Men Regular Fit Track Pants - Cotton Rich - Smart Tech, Easy Stain Release, Anti Stat, Ultra Soft, Quick Dry</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Cantabil</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Enamor</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Essentials Womens Mid Rise 7/8th Relaxed Fit Soft &amp; Drapey 4 Way Stretch Viscose Spandex Lounge Pants with 2 Side Pockets- E048</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Van Heusen</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Athleisure Men Regular Fit Track Pants - Cotton Rich - Smart Tech, Easy Stain Release, Anti Stat, Ultra Soft, Quick Dry</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>hummel</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Enamor</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Women Pants</t>
+        </is>
+      </c>
+      <c r="D123" t="n">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>nexus</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Printed Lounge Pants</t>
+        </is>
+      </c>
+      <c r="D124" t="n">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Enamor</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Essentials Women's Slim Fit Mid Rise Crop Length Soft &amp; Drapey Stretch Viscose Culottes with Smart Side Slits - EA64</t>
+        </is>
+      </c>
+      <c r="D125" t="n">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Jockey</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Mens Slub Casual Track Pant</t>
+        </is>
+      </c>
+      <c r="D126" t="n">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>PETER ENGLAND</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Grey Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D127" t="n">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>BEEVEE</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Men's Cargos</t>
+        </is>
+      </c>
+      <c r="D128" t="n">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>CULTSPORT</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>| AbsoluteFit Abstract Print Tights for Women</t>
+        </is>
+      </c>
+      <c r="D129" t="n">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>rock.it</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D130" t="n">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Speedo</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Contrast Swim Pants</t>
+        </is>
+      </c>
+      <c r="D131" t="n">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>rock.it</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D132" t="n">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Allen Solly</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Grey Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Allen Solly</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Light Blue Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Allen Solly</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Grey Viscose Rayon Trousers</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Allen Solly</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Khaki Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Allen Solly</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Green Cotton Blend Trousers</t>
+        </is>
+      </c>
+      <c r="D137" t="n">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>ONLY</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Women Track Pants</t>
+        </is>
+      </c>
+      <c r="D138" t="n">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Allen Solly</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Grey Viscose Rayon Trousers</t>
+        </is>
+      </c>
+      <c r="D139" t="n">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>United Colors of Benetton</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Light Blue Pure Cotton Trousers</t>
+        </is>
+      </c>
+      <c r="D140" t="n">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Jockey</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D141" t="n">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Puma</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Woven Men'S Training Pants</t>
+        </is>
+      </c>
+      <c r="D142" t="n">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Allen Solly</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Men Slim Fit Blue Viscose Rayon Trousers</t>
+        </is>
+      </c>
+      <c r="D143" t="n">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>The Pant Project</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Luxury PV Lycra Stretchable Formal Pants for Men | Stylish Slim Fit Men's Wear Trousers for Office or Party | Mens Fashion Dress Trouser Pant</t>
+        </is>
+      </c>
+      <c r="D144" t="n">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>The Pant Project</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Luxury PV Stretchable Casual Pants for Men | Stylish Slim Fit Men's Wear Trousers for Office or Party | Mens Fashion Dress Trouser with Expandable Waist &amp; 4 Way Stretch</t>
+        </is>
+      </c>
+      <c r="D145" t="n">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>boohooMAN</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Men Tapered Track Pants</t>
+        </is>
+      </c>
+      <c r="D146" t="n">
+        <v>2249</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>boohooMAN</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>Men Solid Track Pants</t>
+        </is>
+      </c>
+      <c r="D147" t="n">
+        <v>2586</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Puma</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D148" t="n">
+        <v>2799</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>boohooMAN</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>Men Textured Track Pants</t>
+        </is>
+      </c>
+      <c r="D149" t="n">
+        <v>2886</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Puma</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>Men Track Pants</t>
+        </is>
+      </c>
+      <c r="D150" t="n">
+        <v>3199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>